<commit_message>
Linked up column chart to economic indicator selector
</commit_message>
<xml_diff>
--- a/data/economic_data.xlsx
+++ b/data/economic_data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="58">
   <si>
     <t>1_2</t>
   </si>
@@ -191,12 +191,6 @@
     <t>Current $US</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>GDP per Capita</t>
-  </si>
-  <si>
     <t>% of female population ages 15-64</t>
   </si>
   <si>
@@ -204,6 +198,15 @@
   </si>
   <si>
     <t>Female Labor Force Participation Rate</t>
+  </si>
+  <si>
+    <t>Gross Domestic Product</t>
+  </si>
+  <si>
+    <t>Gross Domestic Product per Capita</t>
+  </si>
+  <si>
+    <t>US$</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -524,6 +527,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1088,7 +1094,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,13 +1133,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
         <v>49</v>
@@ -1144,13 +1152,15 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" t="s">
         <v>49</v>
@@ -1161,15 +1171,17 @@
         <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Fixed y-axis on economic indicators chart
</commit_message>
<xml_diff>
--- a/data/economic_data.xlsx
+++ b/data/economic_data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
   <si>
     <t>1_2</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>US$</t>
+  </si>
+  <si>
+    <t>y_axis_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> million</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -528,6 +534,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1091,21 +1100,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1116,19 +1126,22 @@
         <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1138,16 +1151,21 @@
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="9">
+        <v>900000</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1157,16 +1175,19 @@
       <c r="C3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="9">
+        <v>15000</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1176,14 +1197,17 @@
       <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
+        <v>100</v>
+      </c>
+      <c r="E4" s="8">
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1197,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,64 +1301,64 @@
         <v>4</v>
       </c>
       <c r="B2" s="7">
-        <v>3314898291.3775301</v>
+        <v>3314.8982913775303</v>
       </c>
       <c r="C2" s="7">
-        <v>2359903108.2516398</v>
+        <v>2359.9031082516399</v>
       </c>
       <c r="D2" s="7">
-        <v>2707123772.39715</v>
+        <v>2707.1237723971499</v>
       </c>
       <c r="E2" s="7">
-        <v>3414760915.2246399</v>
+        <v>3414.76091522464</v>
       </c>
       <c r="F2" s="7">
-        <v>3632043907.7897401</v>
+        <v>3632.0439077897399</v>
       </c>
       <c r="G2" s="7">
-        <v>4060758804.1064</v>
+        <v>4060.7588041064</v>
       </c>
       <c r="H2" s="7">
-        <v>4435078647.8603897</v>
+        <v>4435.0786478603895</v>
       </c>
       <c r="I2" s="7">
-        <v>5746945912.8856897</v>
+        <v>5746.9459128856897</v>
       </c>
       <c r="J2" s="7">
-        <v>7314865175.6748505</v>
+        <v>7314.8651756748504</v>
       </c>
       <c r="K2" s="7">
-        <v>8158548716.5294104</v>
+        <v>8158.5487165294107</v>
       </c>
       <c r="L2" s="7">
-        <v>8992642348.9579601</v>
+        <v>8992.6423489579593</v>
       </c>
       <c r="M2" s="7">
-        <v>10701011896.7708</v>
+        <v>10701.0118967708</v>
       </c>
       <c r="N2" s="7">
-        <v>12881352687.7773</v>
+        <v>12881.3526877773</v>
       </c>
       <c r="O2" s="7">
-        <v>12044212903.816799</v>
+        <v>12044.212903816799</v>
       </c>
       <c r="P2" s="7">
-        <v>11926953258.916</v>
+        <v>11926.953258916001</v>
       </c>
       <c r="Q2" s="7">
-        <v>12890867538.530199</v>
+        <v>12890.867538530199</v>
       </c>
       <c r="R2" s="7">
-        <v>12319784787.2987</v>
+        <v>12319.7847872987</v>
       </c>
       <c r="S2" s="7">
-        <v>12781029643.593599</v>
+        <v>12781.0296435936</v>
       </c>
       <c r="T2" s="7">
-        <v>13277963807.0823</v>
+        <v>13277.9638070823</v>
       </c>
       <c r="U2" s="7">
-        <v>11455595709.1413</v>
+        <v>11455.5957091413</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -1342,64 +1366,64 @@
         <v>5</v>
       </c>
       <c r="B3" s="7">
-        <v>1596968913.1920199</v>
+        <v>1596.96891319202</v>
       </c>
       <c r="C3" s="7">
-        <v>1639492424.3810301</v>
+        <v>1639.4924243810301</v>
       </c>
       <c r="D3" s="7">
-        <v>1893726437.35976</v>
+        <v>1893.72643735976</v>
       </c>
       <c r="E3" s="7">
-        <v>1845482181.4853899</v>
+        <v>1845.4821814853899</v>
       </c>
       <c r="F3" s="7">
-        <v>1911563665.3900599</v>
+        <v>1911.5636653900599</v>
       </c>
       <c r="G3" s="7">
-        <v>2118467913.3787301</v>
+        <v>2118.4679133787299</v>
       </c>
       <c r="H3" s="7">
-        <v>2376335048.3997598</v>
+        <v>2376.3350483997597</v>
       </c>
       <c r="I3" s="7">
-        <v>2807061008.6908398</v>
+        <v>2807.0610086908396</v>
       </c>
       <c r="J3" s="7">
-        <v>3576615240.4161601</v>
+        <v>3576.6152404161603</v>
       </c>
       <c r="K3" s="7">
-        <v>4900469515.0725203</v>
+        <v>4900.4695150725202</v>
       </c>
       <c r="L3" s="7">
-        <v>6384451606.1421003</v>
+        <v>6384.4516061421</v>
       </c>
       <c r="M3" s="7">
-        <v>9206301700.3961906</v>
+        <v>9206.3017003961904</v>
       </c>
       <c r="N3" s="7">
-        <v>11662040713.875299</v>
+        <v>11662.0407138753</v>
       </c>
       <c r="O3" s="7">
-        <v>8647936747.9870396</v>
+        <v>8647.9367479870398</v>
       </c>
       <c r="P3" s="7">
-        <v>9260284937.7978096</v>
+        <v>9260.2849377978091</v>
       </c>
       <c r="Q3" s="7">
-        <v>10142111334.496099</v>
+        <v>10142.1113344961</v>
       </c>
       <c r="R3" s="7">
-        <v>10619320048.585699</v>
+        <v>10619.3200485857</v>
       </c>
       <c r="S3" s="7">
-        <v>11121465767.4067</v>
+        <v>11121.4657674067</v>
       </c>
       <c r="T3" s="7">
-        <v>11644438422.9844</v>
+        <v>11644.4384229844</v>
       </c>
       <c r="U3" s="7">
-        <v>10561401185.098</v>
+        <v>10561.401185097999</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -1407,64 +1431,64 @@
         <v>6</v>
       </c>
       <c r="B4" s="7">
-        <v>3176749593.1178799</v>
+        <v>3176.7495931178801</v>
       </c>
       <c r="C4" s="7">
-        <v>3962710163.11167</v>
+        <v>3962.7101631116702</v>
       </c>
       <c r="D4" s="7">
-        <v>4446396217.6326504</v>
+        <v>4446.3962176326504</v>
       </c>
       <c r="E4" s="7">
-        <v>4581222442.4578304</v>
+        <v>4581.2224424578308</v>
       </c>
       <c r="F4" s="7">
-        <v>5272617196.0451698</v>
+        <v>5272.6171960451702</v>
       </c>
       <c r="G4" s="7">
-        <v>5707618246.5684795</v>
+        <v>5707.6182465684797</v>
       </c>
       <c r="H4" s="7">
-        <v>6236024951.2042303</v>
+        <v>6236.0249512042301</v>
       </c>
       <c r="I4" s="7">
-        <v>7275766111.2430897</v>
+        <v>7275.7661112430897</v>
       </c>
       <c r="J4" s="7">
-        <v>8680511918.4935703</v>
+        <v>8680.5119184935702</v>
       </c>
       <c r="K4" s="7">
-        <v>13245421880.834</v>
+        <v>13245.421880833999</v>
       </c>
       <c r="L4" s="7">
-        <v>20983019923.886299</v>
+        <v>20983.019923886299</v>
       </c>
       <c r="M4" s="7">
-        <v>33050343782.775902</v>
+        <v>33050.343782775904</v>
       </c>
       <c r="N4" s="7">
-        <v>48852482960.077904</v>
+        <v>48852.482960077905</v>
       </c>
       <c r="O4" s="7">
-        <v>44291490420.502602</v>
+        <v>44291.490420502603</v>
       </c>
       <c r="P4" s="7">
-        <v>52902703376.105598</v>
+        <v>52902.703376105601</v>
       </c>
       <c r="Q4" s="7">
-        <v>65951627200.202599</v>
+        <v>65951.627200202594</v>
       </c>
       <c r="R4" s="7">
-        <v>68730906313.645599</v>
+        <v>68730.906313645595</v>
       </c>
       <c r="S4" s="7">
-        <v>73560484384.958603</v>
+        <v>73560.484384958603</v>
       </c>
       <c r="T4" s="7">
-        <v>75198010965.191895</v>
+        <v>75198.01096519189</v>
       </c>
       <c r="U4" s="7">
-        <v>53047140347.452698</v>
+        <v>53047.140347452696</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1472,64 +1496,64 @@
         <v>7</v>
       </c>
       <c r="B5" s="7">
-        <v>14756861538.4615</v>
+        <v>14756.8615384615</v>
       </c>
       <c r="C5" s="7">
-        <v>14128412417.193001</v>
+        <v>14128.412417193002</v>
       </c>
       <c r="D5" s="7">
-        <v>15222014828.3039</v>
+        <v>15222.0148283039</v>
       </c>
       <c r="E5" s="7">
-        <v>12138485328.626699</v>
+        <v>12138.485328626699</v>
       </c>
       <c r="F5" s="7">
-        <v>12736856485.1068</v>
+        <v>12736.8564851068</v>
       </c>
       <c r="G5" s="7">
-        <v>12354820143.884899</v>
+        <v>12354.820143884899</v>
       </c>
       <c r="H5" s="7">
-        <v>14594925392.969101</v>
+        <v>14594.9253929691</v>
       </c>
       <c r="I5" s="7">
-        <v>17825436034.536598</v>
+        <v>17825.436034536597</v>
       </c>
       <c r="J5" s="7">
-        <v>23141587717.763302</v>
+        <v>23141.587717763301</v>
       </c>
       <c r="K5" s="7">
-        <v>30210091836.829399</v>
+        <v>30210.091836829401</v>
       </c>
       <c r="L5" s="7">
-        <v>36961821893.697601</v>
+        <v>36961.821893697605</v>
       </c>
       <c r="M5" s="7">
-        <v>45275747860.644203</v>
+        <v>45275.747860644202</v>
       </c>
       <c r="N5" s="7">
-        <v>60752177438.889503</v>
+        <v>60752.177438889506</v>
       </c>
       <c r="O5" s="7">
-        <v>49208656976.039001</v>
+        <v>49208.656976039005</v>
       </c>
       <c r="P5" s="7">
-        <v>55220932613.958</v>
+        <v>55220.932613958001</v>
       </c>
       <c r="Q5" s="7">
-        <v>59734593904.640198</v>
+        <v>59734.593904640198</v>
       </c>
       <c r="R5" s="7">
-        <v>63615445566.848297</v>
+        <v>63615.445566848299</v>
       </c>
       <c r="S5" s="7">
-        <v>73097619636.820908</v>
+        <v>73097.619636820906</v>
       </c>
       <c r="T5" s="7">
-        <v>76103961203.440598</v>
+        <v>76103.961203440602</v>
       </c>
       <c r="U5" s="7">
-        <v>54608962634.990799</v>
+        <v>54608.962634990799</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1537,64 +1561,64 @@
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <v>2786045321.6374302</v>
+        <v>2786.0453216374303</v>
       </c>
       <c r="C6" s="7">
-        <v>3671816504.2385101</v>
+        <v>3671.8165042385103</v>
       </c>
       <c r="D6" s="7">
-        <v>4116699437.4040999</v>
+        <v>4116.6994374040996</v>
       </c>
       <c r="E6" s="7">
-        <v>4685729738.5620899</v>
+        <v>4685.7297385620896</v>
       </c>
       <c r="F6" s="7">
-        <v>5505984455.9585505</v>
+        <v>5505.9844559585508</v>
       </c>
       <c r="G6" s="7">
-        <v>5748990666.1786203</v>
+        <v>5748.9906661786199</v>
       </c>
       <c r="H6" s="7">
-        <v>6651226179.0182896</v>
+        <v>6651.2261790182893</v>
       </c>
       <c r="I6" s="7">
-        <v>8370020196.1915798</v>
+        <v>8370.0201961915791</v>
       </c>
       <c r="J6" s="7">
-        <v>10022840634.920601</v>
+        <v>10022.840634920602</v>
       </c>
       <c r="K6" s="7">
-        <v>11225138297.1959</v>
+        <v>11225.138297195899</v>
       </c>
       <c r="L6" s="7">
-        <v>12866524918.222099</v>
+        <v>12866.5249182221</v>
       </c>
       <c r="M6" s="7">
-        <v>15776422673.198</v>
+        <v>15776.422673198</v>
       </c>
       <c r="N6" s="7">
-        <v>19101454463.750702</v>
+        <v>19101.454463750702</v>
       </c>
       <c r="O6" s="7">
-        <v>17600630726.614101</v>
+        <v>17600.630726614101</v>
       </c>
       <c r="P6" s="7">
-        <v>17163117551.462601</v>
+        <v>17163.117551462601</v>
       </c>
       <c r="Q6" s="7">
-        <v>18628022743.425701</v>
+        <v>18628.022743425699</v>
       </c>
       <c r="R6" s="7">
-        <v>17207367625.804798</v>
+        <v>17207.3676258048</v>
       </c>
       <c r="S6" s="7">
-        <v>18154290272.215099</v>
+        <v>18154.290272215101</v>
       </c>
       <c r="T6" s="7">
-        <v>18521476054.809399</v>
+        <v>18521.476054809398</v>
       </c>
       <c r="U6" s="7">
-        <v>15995392117.9473</v>
+        <v>15995.3921179473</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -1602,64 +1626,64 @@
         <v>8</v>
       </c>
       <c r="B7" s="7">
-        <v>3094915505.9092999</v>
+        <v>3094.9155059093</v>
       </c>
       <c r="C7" s="7">
-        <v>3510540809.2485499</v>
+        <v>3510.54080924855</v>
       </c>
       <c r="D7" s="7">
-        <v>3613500117.24928</v>
+        <v>3613.5001172492798</v>
       </c>
       <c r="E7" s="7">
-        <v>2800024313.9514399</v>
+        <v>2800.02431395144</v>
       </c>
       <c r="F7" s="7">
-        <v>3057453482.55826</v>
+        <v>3057.45348255826</v>
       </c>
       <c r="G7" s="7">
-        <v>3219487824.8791099</v>
+        <v>3219.4878248791097</v>
       </c>
       <c r="H7" s="7">
-        <v>3395778673.7918301</v>
+        <v>3395.77867379183</v>
       </c>
       <c r="I7" s="7">
-        <v>3991374548.5051198</v>
+        <v>3991.3745485051199</v>
       </c>
       <c r="J7" s="7">
-        <v>5125273880.74998</v>
+        <v>5125.27388074998</v>
       </c>
       <c r="K7" s="7">
-        <v>6410941012.5918903</v>
+        <v>6410.9410125918903</v>
       </c>
       <c r="L7" s="7">
-        <v>7745406200.8537397</v>
+        <v>7745.4062008537394</v>
       </c>
       <c r="M7" s="7">
-        <v>10172869679.736601</v>
+        <v>10172.869679736601</v>
       </c>
       <c r="N7" s="7">
-        <v>12795044472.7663</v>
+        <v>12795.0444727663</v>
       </c>
       <c r="O7" s="7">
-        <v>10766809099.0721</v>
+        <v>10766.809099072099</v>
       </c>
       <c r="P7" s="7">
-        <v>11638536890.5347</v>
+        <v>11638.5368905347</v>
       </c>
       <c r="Q7" s="7">
-        <v>14434619982.2117</v>
+        <v>14434.6199822117</v>
       </c>
       <c r="R7" s="7">
-        <v>15846474595.773001</v>
+        <v>15846.474595773001</v>
       </c>
       <c r="S7" s="7">
-        <v>16140047072.2616</v>
+        <v>16140.047072261601</v>
       </c>
       <c r="T7" s="7">
-        <v>16509305827.7171</v>
+        <v>16509.3058277171</v>
       </c>
       <c r="U7" s="7">
-        <v>13965385801.789101</v>
+        <v>13965.3858017891</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -1667,64 +1691,64 @@
         <v>11</v>
       </c>
       <c r="B8" s="7">
-        <v>4422160017.5438604</v>
+        <v>4422.1600175438607</v>
       </c>
       <c r="C8" s="7">
-        <v>3735312142.5702801</v>
+        <v>3735.3121425702802</v>
       </c>
       <c r="D8" s="7">
-        <v>3571043102.5640998</v>
+        <v>3571.0431025640996</v>
       </c>
       <c r="E8" s="7">
-        <v>3673288263.6203899</v>
+        <v>3673.2882636203899</v>
       </c>
       <c r="F8" s="7">
-        <v>3772851420.2476301</v>
+        <v>3772.8514202476299</v>
       </c>
       <c r="G8" s="7">
-        <v>3709637829.9486599</v>
+        <v>3709.6378299486601</v>
       </c>
       <c r="H8" s="7">
-        <v>4018365247.4444399</v>
+        <v>4018.3652474444398</v>
       </c>
       <c r="I8" s="7">
-        <v>4946292774.7904596</v>
+        <v>4946.2927747904596</v>
       </c>
       <c r="J8" s="7">
-        <v>5682719260.0762997</v>
+        <v>5682.7192600763001</v>
       </c>
       <c r="K8" s="7">
-        <v>6258600713.8262701</v>
+        <v>6258.6007138262703</v>
       </c>
       <c r="L8" s="7">
-        <v>6861222331.9631701</v>
+        <v>6861.2223319631703</v>
       </c>
       <c r="M8" s="7">
-        <v>8336478142.0887203</v>
+        <v>8336.4781420887211</v>
       </c>
       <c r="N8" s="7">
-        <v>9909548410.8274403</v>
+        <v>9909.5484108274395</v>
       </c>
       <c r="O8" s="7">
-        <v>9401731495.71661</v>
+        <v>9401.7314957166091</v>
       </c>
       <c r="P8" s="7">
-        <v>9407168702.4312992</v>
+        <v>9407.1687024312996</v>
       </c>
       <c r="Q8" s="7">
-        <v>10494632699.3859</v>
+        <v>10494.6326993859</v>
       </c>
       <c r="R8" s="7">
-        <v>9745251126.0109005</v>
+        <v>9745.2511260109004</v>
       </c>
       <c r="S8" s="7">
-        <v>10817712138.945101</v>
+        <v>10817.7121389451</v>
       </c>
       <c r="T8" s="7">
-        <v>11318966946.687</v>
+        <v>11318.966946687</v>
       </c>
       <c r="U8" s="7">
-        <v>10086021260.9944</v>
+        <v>10086.021260994399</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -1732,121 +1756,129 @@
         <v>9</v>
       </c>
       <c r="B9" s="7">
-        <v>21035357832.801899</v>
+        <v>21035.357832801899</v>
       </c>
       <c r="C9" s="7">
-        <v>22165932062.966</v>
+        <v>22165.932062966</v>
       </c>
       <c r="D9" s="7">
-        <v>22135245413.231201</v>
+        <v>22135.245413231201</v>
       </c>
       <c r="E9" s="7">
-        <v>16870817134.776699</v>
+        <v>16870.817134776698</v>
       </c>
       <c r="F9" s="7">
-        <v>18291990619.137001</v>
+        <v>18291.990619137003</v>
       </c>
       <c r="G9" s="7">
-        <v>22152689129.5583</v>
+        <v>22152.689129558301</v>
       </c>
       <c r="H9" s="7">
-        <v>24636598581.020401</v>
+        <v>24636.5985810204</v>
       </c>
       <c r="I9" s="7">
-        <v>30833692831.3955</v>
+        <v>30833.6928313955</v>
       </c>
       <c r="J9" s="7">
-        <v>43151647002.609596</v>
+        <v>43151.647002609599</v>
       </c>
       <c r="K9" s="7">
-        <v>57123671733.895203</v>
+        <v>57123.6717338952</v>
       </c>
       <c r="L9" s="7">
-        <v>81003884545.409897</v>
+        <v>81003.884545409892</v>
       </c>
       <c r="M9" s="7">
-        <v>104849886825.584</v>
+        <v>104849.88682558401</v>
       </c>
       <c r="N9" s="7">
-        <v>133441612246.798</v>
+        <v>133441.612246798</v>
       </c>
       <c r="O9" s="7">
-        <v>115308661142.927</v>
+        <v>115308.661142927</v>
       </c>
       <c r="P9" s="7">
-        <v>148047348240.64301</v>
+        <v>148047.34824064301</v>
       </c>
       <c r="Q9" s="7">
-        <v>200379345222.50601</v>
+        <v>200379.345222506</v>
       </c>
       <c r="R9" s="7">
-        <v>215902443457.121</v>
+        <v>215902.443457121</v>
       </c>
       <c r="S9" s="7">
-        <v>243775211464.992</v>
+        <v>243775.211464992</v>
       </c>
       <c r="T9" s="7">
-        <v>227437054841.26801</v>
+        <v>227437.05484126799</v>
       </c>
       <c r="U9" s="7">
-        <v>184360630555.504</v>
+        <v>184360.630555504</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
       <c r="F10" s="7">
-        <v>1849196082.0550699</v>
+        <v>1849.1960820550698</v>
       </c>
       <c r="G10" s="7">
-        <v>2535333631.8853598</v>
+        <v>2535.3336318853599</v>
       </c>
       <c r="H10" s="7">
-        <v>2702427046.9355001</v>
+        <v>2702.4270469355001</v>
       </c>
       <c r="I10" s="7">
-        <v>3355083116.5893898</v>
+        <v>3355.0831165893896</v>
       </c>
       <c r="J10" s="7">
-        <v>3639935347.5071502</v>
+        <v>3639.9353475071503</v>
       </c>
       <c r="K10" s="7">
-        <v>3736599925.38241</v>
+        <v>3736.5999253824102</v>
       </c>
       <c r="L10" s="7">
-        <v>4078158323.9242301</v>
+        <v>4078.15832392423</v>
       </c>
       <c r="M10" s="7">
-        <v>4833561456.3372602</v>
+        <v>4833.5614563372601</v>
       </c>
       <c r="N10" s="7">
-        <v>5687488208.58356</v>
+        <v>5687.4882085835598</v>
       </c>
       <c r="O10" s="7">
-        <v>5653792720.2000599</v>
+        <v>5653.7927202000601</v>
       </c>
       <c r="P10" s="7">
-        <v>5829933774.8344402</v>
+        <v>5829.9337748344406</v>
       </c>
       <c r="Q10" s="7">
-        <v>6692521545.7325497</v>
+        <v>6692.5215457325494</v>
       </c>
       <c r="R10" s="7">
-        <v>6500321212.89991</v>
+        <v>6500.3212128999103</v>
       </c>
       <c r="S10" s="7">
-        <v>7073021773.7652702</v>
+        <v>7073.0217737652702</v>
       </c>
       <c r="T10" s="7">
-        <v>7384901154.3054304</v>
+        <v>7384.9011543054303</v>
       </c>
       <c r="U10" s="7">
-        <v>6385937673.2838001</v>
+        <v>6385.9376732838</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -1854,64 +1886,64 @@
         <v>21</v>
       </c>
       <c r="B11" s="7">
-        <v>1827570586.16784</v>
+        <v>1827.57058616784</v>
       </c>
       <c r="C11" s="7">
-        <v>1767864035.71943</v>
+        <v>1767.8640357194299</v>
       </c>
       <c r="D11" s="7">
-        <v>1645963749.83146</v>
+        <v>1645.9637498314601</v>
       </c>
       <c r="E11" s="7">
-        <v>1249062025.1380501</v>
+        <v>1249.0620251380501</v>
       </c>
       <c r="F11" s="7">
-        <v>1369691955.02213</v>
+        <v>1369.6919550221301</v>
       </c>
       <c r="G11" s="7">
-        <v>1525113501.1103401</v>
+        <v>1525.1135011103402</v>
       </c>
       <c r="H11" s="7">
-        <v>1605640633.42189</v>
+        <v>1605.64063342189</v>
       </c>
       <c r="I11" s="7">
-        <v>1919012780.97086</v>
+        <v>1919.0127809708599</v>
       </c>
       <c r="J11" s="7">
-        <v>2211535311.6283398</v>
+        <v>2211.53531162834</v>
       </c>
       <c r="K11" s="7">
-        <v>2460246796.05234</v>
+        <v>2460.24679605234</v>
       </c>
       <c r="L11" s="7">
-        <v>2834168889.4201899</v>
+        <v>2834.1688894201898</v>
       </c>
       <c r="M11" s="7">
-        <v>3802566170.8154302</v>
+        <v>3802.5661708154303</v>
       </c>
       <c r="N11" s="7">
-        <v>5139957784.91084</v>
+        <v>5139.95778491084</v>
       </c>
       <c r="O11" s="7">
-        <v>4690062255.1224699</v>
+        <v>4690.0622551224697</v>
       </c>
       <c r="P11" s="7">
-        <v>4794357795.0713902</v>
+        <v>4794.3577950713898</v>
       </c>
       <c r="Q11" s="7">
-        <v>6197766118.5985603</v>
+        <v>6197.7661185985608</v>
       </c>
       <c r="R11" s="7">
-        <v>6605139933.4106302</v>
+        <v>6605.13993341063</v>
       </c>
       <c r="S11" s="7">
-        <v>7335027591.9162798</v>
+        <v>7335.0275919162796</v>
       </c>
       <c r="T11" s="7">
-        <v>7468096566.7115803</v>
+        <v>7468.0965667115806</v>
       </c>
       <c r="U11" s="7">
-        <v>6571853849.0058498</v>
+        <v>6571.85384900585</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -1919,121 +1951,129 @@
         <v>12</v>
       </c>
       <c r="B12" s="7">
-        <v>1695130456.52174</v>
+        <v>1695.1304565217399</v>
       </c>
       <c r="C12" s="7">
-        <v>1930071406.92641</v>
+        <v>1930.07140692641</v>
       </c>
       <c r="D12" s="7">
-        <v>1639497206.7039101</v>
+        <v>1639.49720670391</v>
       </c>
       <c r="E12" s="7">
-        <v>1170785047.79461</v>
+        <v>1170.7850477946101</v>
       </c>
       <c r="F12" s="7">
-        <v>1288420222.94787</v>
+        <v>1288.4202229478701</v>
       </c>
       <c r="G12" s="7">
-        <v>1480656884.38462</v>
+        <v>1480.6568843846198</v>
       </c>
       <c r="H12" s="7">
-        <v>1661818168.4226</v>
+        <v>1661.8181684226001</v>
       </c>
       <c r="I12" s="7">
-        <v>1980901553.51226</v>
+        <v>1980.9015535122599</v>
       </c>
       <c r="J12" s="7">
-        <v>2598231467.4367099</v>
+        <v>2598.2314674367099</v>
       </c>
       <c r="K12" s="7">
-        <v>2988338439.3155298</v>
+        <v>2988.3384393155297</v>
       </c>
       <c r="L12" s="7">
-        <v>3408272498.11516</v>
+        <v>3408.27249811516</v>
       </c>
       <c r="M12" s="7">
-        <v>4401154128.1229696</v>
+        <v>4401.1541281229693</v>
       </c>
       <c r="N12" s="7">
-        <v>6054806100.8467999</v>
+        <v>6054.8061008468003</v>
       </c>
       <c r="O12" s="7">
-        <v>5439422031.3962698</v>
+        <v>5439.4220313962696</v>
       </c>
       <c r="P12" s="7">
-        <v>5811604051.96737</v>
+        <v>5811.6040519673697</v>
       </c>
       <c r="Q12" s="7">
-        <v>7015206498.2195501</v>
+        <v>7015.2064982195498</v>
       </c>
       <c r="R12" s="7">
-        <v>7284686576.2834997</v>
+        <v>7284.6865762834996</v>
       </c>
       <c r="S12" s="7">
-        <v>7985349731.4647102</v>
+        <v>7985.3497314647102</v>
       </c>
       <c r="T12" s="7">
-        <v>7983271110.6044598</v>
+        <v>7983.2711106044599</v>
       </c>
       <c r="U12" s="7">
-        <v>6551161404.0935698</v>
+        <v>6551.1614040935701</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
       <c r="F13" s="7">
-        <v>984279598.32525098</v>
+        <v>984.27959832525096</v>
       </c>
       <c r="G13" s="7">
-        <v>1159891557.1698599</v>
+        <v>1159.8915571698599</v>
       </c>
       <c r="H13" s="7">
-        <v>1284504507.6985099</v>
+        <v>1284.50450769851</v>
       </c>
       <c r="I13" s="7">
-        <v>1707662612.68399</v>
+        <v>1707.6626126839899</v>
       </c>
       <c r="J13" s="7">
-        <v>2073255525.20487</v>
+        <v>2073.2555252048701</v>
       </c>
       <c r="K13" s="7">
-        <v>2257118340.5461898</v>
+        <v>2257.1183405461898</v>
       </c>
       <c r="L13" s="7">
-        <v>2696020574.58286</v>
+        <v>2696.0205745828598</v>
       </c>
       <c r="M13" s="7">
-        <v>3668857103.75034</v>
+        <v>3668.8571037503398</v>
       </c>
       <c r="N13" s="7">
-        <v>4519731946.6822901</v>
+        <v>4519.7319466822901</v>
       </c>
       <c r="O13" s="7">
-        <v>4141382328.4245601</v>
+        <v>4141.38232842456</v>
       </c>
       <c r="P13" s="7">
-        <v>4139192052.9801302</v>
+        <v>4139.19205298013</v>
       </c>
       <c r="Q13" s="7">
-        <v>4538199888.7962198</v>
+        <v>4538.19988879622</v>
       </c>
       <c r="R13" s="7">
-        <v>4087725812.6686401</v>
+        <v>4087.7258126686402</v>
       </c>
       <c r="S13" s="7">
-        <v>4464497583.5147896</v>
+        <v>4464.4975835147898</v>
       </c>
       <c r="T13" s="7">
-        <v>4587741791.10639</v>
+        <v>4587.7417911063903</v>
       </c>
       <c r="U13" s="7">
-        <v>3992640233.1701899</v>
+        <v>3992.6402331701897</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -2041,64 +2081,64 @@
         <v>14</v>
       </c>
       <c r="B14" s="7">
-        <v>20948677839.851002</v>
+        <v>20948.677839851003</v>
       </c>
       <c r="C14" s="7">
-        <v>24147996549.5662</v>
+        <v>24147.9965495662</v>
       </c>
       <c r="D14" s="7">
-        <v>18284194680.384399</v>
+        <v>18284.1946803844</v>
       </c>
       <c r="E14" s="7">
-        <v>18409364146.979401</v>
+        <v>18409.364146979402</v>
       </c>
       <c r="F14" s="7">
-        <v>6540247190.33529</v>
+        <v>6540.2471903352898</v>
       </c>
       <c r="G14" s="7">
-        <v>12267175481.2542</v>
+        <v>12267.1754812542</v>
       </c>
       <c r="H14" s="7">
-        <v>16116843146.4806</v>
+        <v>16116.8431464806</v>
       </c>
       <c r="I14" s="7">
-        <v>21188704081.242802</v>
+        <v>21188.704081242802</v>
       </c>
       <c r="J14" s="7">
-        <v>24861483280.6339</v>
+        <v>24861.4832806339</v>
       </c>
       <c r="K14" s="7">
-        <v>26252007830.463902</v>
+        <v>26252.007830463903</v>
       </c>
       <c r="L14" s="7">
-        <v>30607991862.484299</v>
+        <v>30607.991862484298</v>
       </c>
       <c r="M14" s="7">
-        <v>40289556656.1455</v>
+        <v>40289.556656145498</v>
       </c>
       <c r="N14" s="7">
-        <v>49259526052.742599</v>
+        <v>49259.5260527426</v>
       </c>
       <c r="O14" s="7">
-        <v>42616653299.911499</v>
+        <v>42616.653299911501</v>
       </c>
       <c r="P14" s="7">
-        <v>39460357730.5224</v>
+        <v>39460.357730522403</v>
       </c>
       <c r="Q14" s="7">
-        <v>46466728666.610298</v>
+        <v>46466.728666610295</v>
       </c>
       <c r="R14" s="7">
-        <v>40742313861.137398</v>
+        <v>40742.313861137394</v>
       </c>
       <c r="S14" s="7">
-        <v>45519650911.413803</v>
+        <v>45519.650911413803</v>
       </c>
       <c r="T14" s="7">
-        <v>44210806365.681702</v>
+        <v>44210.806365681703</v>
       </c>
       <c r="U14" s="7">
-        <v>36513027127.672302</v>
+        <v>36513.0271276723</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -2106,64 +2146,64 @@
         <v>15</v>
       </c>
       <c r="B15" s="7">
-        <v>1043893062.60575</v>
+        <v>1043.8930626057499</v>
       </c>
       <c r="C15" s="7">
-        <v>921843115.77449799</v>
+        <v>921.84311577449796</v>
       </c>
       <c r="D15" s="7">
-        <v>1320126664.94978</v>
+        <v>1320.12666494978</v>
       </c>
       <c r="E15" s="7">
-        <v>1086567367.91081</v>
+        <v>1086.5673679108099</v>
       </c>
       <c r="F15" s="7">
-        <v>860550294.27346694</v>
+        <v>860.55029427346699</v>
       </c>
       <c r="G15" s="7">
-        <v>1080774005.56446</v>
+        <v>1080.7740055644601</v>
       </c>
       <c r="H15" s="7">
-        <v>1221113794.72523</v>
+        <v>1221.11379472523</v>
       </c>
       <c r="I15" s="7">
-        <v>1554125542.5622301</v>
+        <v>1554.1255425622301</v>
       </c>
       <c r="J15" s="7">
-        <v>2076148710.31813</v>
+        <v>2076.1487103181298</v>
       </c>
       <c r="K15" s="7">
-        <v>2312344310.51263</v>
+        <v>2312.3443105126298</v>
       </c>
       <c r="L15" s="7">
-        <v>2830228903.33498</v>
+        <v>2830.2289033349798</v>
       </c>
       <c r="M15" s="7">
-        <v>3719515378.9177098</v>
+        <v>3719.5153789177098</v>
       </c>
       <c r="N15" s="7">
-        <v>5161298559.3424101</v>
+        <v>5161.29855934241</v>
       </c>
       <c r="O15" s="7">
-        <v>4979471963.7922001</v>
+        <v>4979.4719637921999</v>
       </c>
       <c r="P15" s="7">
-        <v>5642221528.6707201</v>
+        <v>5642.2215286707205</v>
       </c>
       <c r="Q15" s="7">
-        <v>6522755783.3930302</v>
+        <v>6522.7557833930305</v>
       </c>
       <c r="R15" s="7">
-        <v>7633036366.03545</v>
+        <v>7633.0363660354496</v>
       </c>
       <c r="S15" s="7">
-        <v>8506674782.7547102</v>
+        <v>8506.6747827547097</v>
       </c>
       <c r="T15" s="7">
-        <v>9236309138.0427704</v>
+        <v>9236.3091380427704</v>
       </c>
       <c r="U15" s="7">
-        <v>7853450374.0001001</v>
+        <v>7853.4503740001001</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -2171,64 +2211,64 @@
         <v>16</v>
       </c>
       <c r="B16" s="7">
-        <v>181475555282.55499</v>
+        <v>181475.555282555</v>
       </c>
       <c r="C16" s="7">
-        <v>189834649111.25699</v>
+        <v>189834.64911125699</v>
       </c>
       <c r="D16" s="7">
-        <v>269287100882.23999</v>
+        <v>269287.10088223999</v>
       </c>
       <c r="E16" s="7">
-        <v>249751469675.263</v>
+        <v>249751.46967526301</v>
       </c>
       <c r="F16" s="7">
-        <v>266567532789.50699</v>
+        <v>266567.53278950701</v>
       </c>
       <c r="G16" s="7">
-        <v>196005289735.64001</v>
+        <v>196005.28973564002</v>
       </c>
       <c r="H16" s="7">
-        <v>232534560443.20599</v>
+        <v>232534.56044320599</v>
       </c>
       <c r="I16" s="7">
-        <v>303005303084.81598</v>
+        <v>303005.30308481597</v>
       </c>
       <c r="J16" s="7">
-        <v>392166275622.58899</v>
+        <v>392166.27562258899</v>
       </c>
       <c r="K16" s="7">
-        <v>482979839089.01501</v>
+        <v>482979.83908901503</v>
       </c>
       <c r="L16" s="7">
-        <v>530900094644.73199</v>
+        <v>530900.09464473196</v>
       </c>
       <c r="M16" s="7">
-        <v>647155131629.44202</v>
+        <v>647155.13162944198</v>
       </c>
       <c r="N16" s="7">
-        <v>730337495197.849</v>
+        <v>730337.495197849</v>
       </c>
       <c r="O16" s="7">
-        <v>614553921935.48401</v>
+        <v>614553.92193548405</v>
       </c>
       <c r="P16" s="7">
-        <v>731168051636.94397</v>
+        <v>731168.05163694394</v>
       </c>
       <c r="Q16" s="7">
-        <v>774754155820.89502</v>
+        <v>774754.15582089499</v>
       </c>
       <c r="R16" s="7">
-        <v>788863301224.94397</v>
+        <v>788863.30122494395</v>
       </c>
       <c r="S16" s="7">
-        <v>823242587456.66602</v>
+        <v>823242.58745666605</v>
       </c>
       <c r="T16" s="7">
-        <v>798797266164.03894</v>
+        <v>798797.26616403891</v>
       </c>
       <c r="U16" s="7">
-        <v>718221078308.82397</v>
+        <v>718221.07830882398</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -2236,64 +2276,64 @@
         <v>17</v>
       </c>
       <c r="B17" s="7">
-        <v>2379281767.9558001</v>
+        <v>2379.2817679558002</v>
       </c>
       <c r="C17" s="7">
-        <v>2450084970.2474098</v>
+        <v>2450.0849702474097</v>
       </c>
       <c r="D17" s="7">
-        <v>2605688065.0833802</v>
+        <v>2605.68806508338</v>
       </c>
       <c r="E17" s="7">
-        <v>2450686659.7779899</v>
+        <v>2450.6866597779899</v>
       </c>
       <c r="F17" s="7">
-        <v>2904662604.8205299</v>
+        <v>2904.6626048205299</v>
       </c>
       <c r="G17" s="7">
-        <v>3534771968.5118899</v>
+        <v>3534.77196851189</v>
       </c>
       <c r="H17" s="7">
-        <v>4462028988.7294903</v>
+        <v>4462.0289887294903</v>
       </c>
       <c r="I17" s="7">
-        <v>5977440582.8017101</v>
+        <v>5977.4405828017098</v>
       </c>
       <c r="J17" s="7">
-        <v>6838351088.4668798</v>
+        <v>6838.3510884668794</v>
       </c>
       <c r="K17" s="7">
-        <v>8104355716.8783998</v>
+        <v>8104.3557168784</v>
       </c>
       <c r="L17" s="7">
-        <v>10277598152.4249</v>
+        <v>10277.5981524249</v>
       </c>
       <c r="M17" s="7">
-        <v>12664165103.189501</v>
+        <v>12664.165103189502</v>
       </c>
       <c r="N17" s="7">
-        <v>19271523178.807899</v>
+        <v>19271.5231788079</v>
       </c>
       <c r="O17" s="7">
-        <v>20214385964.9123</v>
+        <v>20214.385964912301</v>
       </c>
       <c r="P17" s="7">
-        <v>22583157894.736801</v>
+        <v>22583.1578947368</v>
       </c>
       <c r="Q17" s="7">
-        <v>29233333333.333302</v>
+        <v>29233.333333333303</v>
       </c>
       <c r="R17" s="7">
-        <v>35164210526.315804</v>
+        <v>35164.210526315801</v>
       </c>
       <c r="S17" s="7">
-        <v>39197543859.649101</v>
+        <v>39197.5438596491</v>
       </c>
       <c r="T17" s="7">
-        <v>43485614035.0877</v>
+        <v>43485.614035087703</v>
       </c>
       <c r="U17" s="7">
-        <v>37334232257.142899</v>
+        <v>37334.232257142896</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
@@ -2301,64 +2341,64 @@
         <v>18</v>
       </c>
       <c r="B18" s="7">
-        <v>44558076851.598801</v>
+        <v>44558.076851598802</v>
       </c>
       <c r="C18" s="7">
-        <v>50150401353.601501</v>
+        <v>50150.401353601505</v>
       </c>
       <c r="D18" s="7">
-        <v>41883242906.715698</v>
+        <v>41883.242906715699</v>
       </c>
       <c r="E18" s="7">
-        <v>31580961262.831699</v>
+        <v>31580.961262831701</v>
       </c>
       <c r="F18" s="7">
-        <v>31261718319.179401</v>
+        <v>31261.718319179403</v>
       </c>
       <c r="G18" s="7">
-        <v>38009344576.608803</v>
+        <v>38009.344576608804</v>
       </c>
       <c r="H18" s="7">
-        <v>42392896031.239403</v>
+        <v>42392.896031239405</v>
       </c>
       <c r="I18" s="7">
-        <v>50132953288.203003</v>
+        <v>50132.953288203003</v>
       </c>
       <c r="J18" s="7">
-        <v>64883060725.700302</v>
+        <v>64883.060725700299</v>
       </c>
       <c r="K18" s="7">
-        <v>86142018069.350403</v>
+        <v>86142.018069350408</v>
       </c>
       <c r="L18" s="7">
-        <v>107753069306.931</v>
+        <v>107753.06930693099</v>
       </c>
       <c r="M18" s="7">
-        <v>142719009900.98999</v>
+        <v>142719.00990099</v>
       </c>
       <c r="N18" s="7">
-        <v>179992405832.32101</v>
+        <v>179992.405832321</v>
       </c>
       <c r="O18" s="7">
-        <v>117227769791.56</v>
+        <v>117227.76979156</v>
       </c>
       <c r="P18" s="7">
-        <v>136419300367.96201</v>
+        <v>136419.30036796202</v>
       </c>
       <c r="Q18" s="7">
-        <v>163159671670.26501</v>
+        <v>163159.671670265</v>
       </c>
       <c r="R18" s="7">
-        <v>175781379051.43301</v>
+        <v>175781.379051433</v>
       </c>
       <c r="S18" s="7">
-        <v>181334417615.41299</v>
+        <v>181334.417615413</v>
       </c>
       <c r="T18" s="7">
-        <v>131805126738.287</v>
+        <v>131805.12673828701</v>
       </c>
       <c r="U18" s="7">
-        <v>90615023323.735306</v>
+        <v>90615.02332373531</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
@@ -2366,64 +2406,64 @@
         <v>19</v>
       </c>
       <c r="B19" s="7">
-        <v>13948892215.568899</v>
+        <v>13948.8922155689</v>
       </c>
       <c r="C19" s="7">
-        <v>14744603773.5849</v>
+        <v>14744.6037735849</v>
       </c>
       <c r="D19" s="7">
-        <v>14988971210.838301</v>
+        <v>14988.971210838301</v>
       </c>
       <c r="E19" s="7">
-        <v>17078465982.0282</v>
+        <v>17078.4659820282</v>
       </c>
       <c r="F19" s="7">
-        <v>13760374487.51</v>
+        <v>13760.37448751</v>
       </c>
       <c r="G19" s="7">
-        <v>11401351420.171801</v>
+        <v>11401.351420171801</v>
       </c>
       <c r="H19" s="7">
-        <v>9687951055.2254105</v>
+        <v>9687.9510552254105</v>
       </c>
       <c r="I19" s="7">
-        <v>10128112401.424801</v>
+        <v>10128.112401424802</v>
       </c>
       <c r="J19" s="7">
-        <v>12030023547.880699</v>
+        <v>12030.023547880699</v>
       </c>
       <c r="K19" s="7">
-        <v>14307509838.8053</v>
+        <v>14307.509838805299</v>
       </c>
       <c r="L19" s="7">
-        <v>17030896203.196301</v>
+        <v>17030.896203196302</v>
       </c>
       <c r="M19" s="7">
-        <v>22311393927.881699</v>
+        <v>22311.393927881698</v>
       </c>
       <c r="N19" s="7">
-        <v>27934030937.215698</v>
+        <v>27934.030937215699</v>
       </c>
       <c r="O19" s="7">
-        <v>32816828372.9753</v>
+        <v>32816.828372975302</v>
       </c>
       <c r="P19" s="7">
-        <v>39332770928.942596</v>
+        <v>39332.770928942598</v>
       </c>
       <c r="Q19" s="7">
-        <v>45324319955.388397</v>
+        <v>45324.319955388397</v>
       </c>
       <c r="R19" s="7">
-        <v>51183443224.993896</v>
+        <v>51183.443224993898</v>
       </c>
       <c r="S19" s="7">
-        <v>56795656324.582298</v>
+        <v>56795.656324582298</v>
       </c>
       <c r="T19" s="7">
-        <v>63132848445.013298</v>
+        <v>63132.848445013296</v>
       </c>
       <c r="U19" s="7">
-        <v>66732801392.661797</v>
+        <v>66732.8013926618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new line chart to Country view
</commit_message>
<xml_diff>
--- a/data/economic_data.xlsx
+++ b/data/economic_data.xlsx
@@ -1257,7 +1257,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1307,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="D2" s="14">
         <v>900000</v>

</xml_diff>